<commit_message>
caught up with journal
</commit_message>
<xml_diff>
--- a/cheese_ratings.xlsx
+++ b/cheese_ratings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/alh328_cornell_edu/Documents/Desktop/cheesepics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1386" documentId="8_{08416551-8C11-4CEF-8EC3-4808968D2082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{162D668A-200C-4638-BC01-34D6DE0D5420}"/>
+  <xr:revisionPtr revIDLastSave="1645" documentId="8_{08416551-8C11-4CEF-8EC3-4808968D2082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5BFAF7-AD23-40B2-9A0C-6EDC103D483E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{E25DB08D-19CD-41DE-9728-FE593DF0F725}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E25DB08D-19CD-41DE-9728-FE593DF0F725}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="608">
   <si>
     <t>maker</t>
   </si>
@@ -488,9 +488,6 @@
     <t>Mozzarella</t>
   </si>
   <si>
-    <t>Homemade with Baggio Evangelista &amp; Joey Ragusa, Jr., along with Carli Opland &amp; Giulia Fragola</t>
-  </si>
-  <si>
     <t>Served slightly warmed, with olive oil, salt, pepper. Creamy, rich, tasty. Texture not exactly correct - needed more stretch. Still delish, must do again.</t>
   </si>
   <si>
@@ -617,9 +614,6 @@
     <t>Italy</t>
   </si>
   <si>
-    <t>Giulia Fragola</t>
-  </si>
-  <si>
     <t>Oh golly gee this is amazing cheese. Hard, aged cheese with a large crumbly texture. Nutty, rich, creamy and also salty and buttery. Great alone, on a tomato sauce dish too… yummm</t>
   </si>
   <si>
@@ -665,15 +659,9 @@
     <t>Quite rich and creamy, soft but "sticker" texture than other Taleggio. I wish it had a firmer rind like the other. Tastes fairly funky and quite salty. Feels a bit one dimensional compared to the other Taleggio.</t>
   </si>
   <si>
-    <t>Julia's uncle</t>
-  </si>
-  <si>
     <t>Caciacavallo</t>
   </si>
   <si>
-    <t>Julia's Uncle</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shaped like a bell with a top knob thing. Tan with a layered waxy rind. Salty, dry, umami. Tastes remarkably like salami - aged, meaty. Most unique cheese thus far for me - addictive. </t>
   </si>
   <si>
@@ -1599,6 +1587,279 @@
   </si>
   <si>
     <t>Face-Rock-Creamery_vampire-slayer2</t>
+  </si>
+  <si>
+    <t>Harbison Spruce Bark-Wrapped Bloomy Rind Cheese</t>
+  </si>
+  <si>
+    <t>Soft white/tan creamy cheese wrapped in leathery bark. Complex funky yet sweet/caramel flavor. Not salty, tastes rich &amp; fattry, also mushroomy, barky. Designed to pair with Rasberry Mostarda jam/mustard combo, which is amazing (separate &amp; together). Unique, hard to rate, subtle &amp; tasty but not my usual style. I respect this cheese.</t>
+  </si>
+  <si>
+    <t>Milky, buttery, salty taste, a bit sweet. Smells very funky but taste is surprisingly mild (note: other bites funkier). Interesting texture prile - light and gooey, almost slimy center, with chewy exterior. Very nice pairing with mustard raspberry jam.</t>
+  </si>
+  <si>
+    <t>Cheeses_-_Harbison_2_of_2</t>
+  </si>
+  <si>
+    <t>Creamy soft white cheese, looks like brie. Very mild, only slight funk, very buttery and creamy. Great with a spicy jam, or the raspberry mustard stuff. For brie and me, it's good!</t>
+  </si>
+  <si>
+    <t>Supper buttery/creamy, rich, salty. Fairly mild, a bit of funk up front but dissapates quickly into butter. Nice texture, medium soft, not too runny, with a bit of chewy rind.</t>
+  </si>
+  <si>
+    <t>Cave-Ripened Mild Brie</t>
+  </si>
+  <si>
+    <t>b042fd9c17daffd4574c125b3057f3982390569b</t>
+  </si>
+  <si>
+    <t>Barb Necarsulmer: Smooth, creamy, buttery. 4.5/5; Rob Necarsulmer: Creamy, very mild and smooth. 4.0/5</t>
+  </si>
+  <si>
+    <t>Barb Necarsulmer: A bit funky, sprice wrapped, mushroomy. 3.8/5</t>
+  </si>
+  <si>
+    <t>Barb Necarsulmer: A bit garlicky, but mild, semi soft. Interesting. 2.8/5</t>
+  </si>
+  <si>
+    <t>Brugge</t>
+  </si>
+  <si>
+    <t>Comtesse Gouda</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Hard tan cheese with a dark blue waxy rind. Nutty, caramelly gouda with salt crystals throughout. Tastes aged, sharper than many goudas. Dries out easily - near rind becomes very hard. Average cheese but very snackable.</t>
+  </si>
+  <si>
+    <t>Nutty, caramelly, a bit salty/sweet. Nice Gouda flavor, but not a fan of the gummy texture. Definitely snackable but not remarkable.</t>
+  </si>
+  <si>
+    <t>sfeer_brugge_comtesse_hor</t>
+  </si>
+  <si>
+    <t>Cottonseed</t>
+  </si>
+  <si>
+    <t>Soft white ripe cheese that was still a tiny bit firm in the center (not 100% ripe). Creamy, salty, taste up front, then the funk comes up the nose/throat. Rind especially funky, but overall pretty mild. Not as buttery as some Brie-like cheeses. Note: rated while grumpy/tired.</t>
+  </si>
+  <si>
+    <t>Tasty Brie-like cheese, buttery, pretty mild but a nice bit of funk. A bit firmer than typical brie, which I like. But still soft &amp; gooey center, chewier rind. Not remarkable but I like Brie.</t>
+  </si>
+  <si>
+    <t>Boxcarr-Cheese</t>
+  </si>
+  <si>
+    <t>Ponce de Leon</t>
+  </si>
+  <si>
+    <t>Pale tan firm with classic striped brown/purple rind. Nutty, salty, buttery cheese, a bit of caramel aftertaste, but also meaty? Very snackable - not an excellent Manchego (2.0/5), but still very tasty in general.</t>
+  </si>
+  <si>
+    <t>Salty, buttery, tangy, bright, and semi sharp. Sort of firm, a bit crumbly. So snackable, could (no, did) eat a lot of this.</t>
+  </si>
+  <si>
+    <t>poncedeleon</t>
+  </si>
+  <si>
+    <t>Valut 5 Cave-Aged Cheddar</t>
+  </si>
+  <si>
+    <t>Tan brown hard cheese with rind that looks like brown salt and pepper. Nutty and woodsy and a teeny bit of funky flavor. Not very salty or buttery. I would not have guessed this was a Cheddar in any world. Definitely dries out.</t>
+  </si>
+  <si>
+    <t>Light brown, slightly orange, pretty hard. Looks more like an aged Gouda than Cheddar. Nutty and pretty funky. Just a touch of Cheddar sharpness, and a bit of Gouda caramel notes. Weird funky aftertaste. After note: apparently this includes Alphine-style cultures, which gives it its not-that-cheddary taste.</t>
+  </si>
+  <si>
+    <t>Cheese_Vault_5_600x480</t>
+  </si>
+  <si>
+    <t>Firm yellowy-tan cheese with a flaky, cakey, brown and white rind. Very grassy, a bit staticky/funky taste, especially at the rind. Some nutty and woodsy flavor, some aged Comte vibes. Not a great melty cheese nor is it super snackable…</t>
+  </si>
+  <si>
+    <t>Nutty, semi sweet, almost meaty flavor in interior, quite funky/barny rind. Really nice semi firm, smooth, chewy texture. I think this one is quite snackable, at least in center.</t>
+  </si>
+  <si>
+    <t>Casatica di Bufala</t>
+  </si>
+  <si>
+    <t>Soft white cheese with a grayish moldy looking rind. Bitter with a bummy fresh mozzarella-y texture. Way down tastes kind of buttery and sweet like Brie but overtop of it it's just bitter. But maybe ours is bad or old. A little funky too. Not my favorite, was better when first opened but still not my favorite.</t>
+  </si>
+  <si>
+    <t>I really don't like this one. Flavor is a mix of metallic bitterness and funky barn dirt. Some creamy Brie in there somewhere but hard to find. Interior is unpleasant gummy texture and rind is unpleasant crumbly texture. The Wegmans guy said it was nice warmed up as a spread, which we didn't try, to be fair. But I doubt it.</t>
+  </si>
+  <si>
+    <t>a14ebac6bde044aa824200bbf485cc0f</t>
+  </si>
+  <si>
+    <t>Italian Truffle Cheese</t>
+  </si>
+  <si>
+    <t>Firm off white cheese with brown mini mushroom looking flakes. It's got a bummy texture and a very rich buttery garlicky mushroom flavor. A little salty but not too much. It's tasty but a little too rich for me to eat a whole block.</t>
+  </si>
+  <si>
+    <t>Rich buttery truffley flavor, nicely integrated into the cheese. It's hard to tell if the cheese itself is quality below the truffle if that makes sense. Seems like a sort of standard Monterrey Jack type. It's tasty and snackable but maybe a bit cheating. Semi firm semi chewy, unremarkable texture.</t>
+  </si>
+  <si>
+    <t>tjtruffle</t>
+  </si>
+  <si>
+    <t>Istara</t>
+  </si>
+  <si>
+    <t>P'Tit Basque Sheep's Milk Cheese</t>
+  </si>
+  <si>
+    <t>Tan cheese (pale, off white) with a light brown patterned rind. Firm cheese, dry texture, but not in a bad way. Mild flavor, nutty, not salty, a mild caramel flavor. Tastes a bit like a Cheddar. Very snackable and tasty.</t>
+  </si>
+  <si>
+    <t>Nutty, creamy, slightly sweet, slightly sharp, just a tiny hint of funk if you look for it (more on rind), but pretty mild overall. Taste reminds me of Manchego a bit, but texture more chewy. Supremely snackable.</t>
+  </si>
+  <si>
+    <t>ptitbasque</t>
+  </si>
+  <si>
+    <t>Spanish Manchego</t>
+  </si>
+  <si>
+    <t>Tan offwhite firm cheese with a stripy red waxy rind. Kind of crumbly texture. Buttery grassy taste, a little bit of nuttiness as well. Not the best Manchego I've ever had but it is incredibly snackable and I could eat a whole block in one sitting if I didn't throw up first.</t>
+  </si>
+  <si>
+    <t>Has that classic tangy, milky Manchego taste, with a bit of grassiness on the finish. Crumbly chewy texture, with waxy rind adding nice bit of firmness. This one has dried out a bit since we got it. Not the peak Manchego but still very snackable.</t>
+  </si>
+  <si>
+    <t>manchego-anejo-cheese</t>
+  </si>
+  <si>
+    <t>Artikaas</t>
+  </si>
+  <si>
+    <t>Clarina Vintage 36-Month Old Gouda</t>
+  </si>
+  <si>
+    <t>Hard pale orange cheese with a orange brown waxy rind. Solid but kind of crumbly texture with some large salty cheese crystals throughout. A salty caramely nutty flavor that is very sharp and aged tasting. Tastes a bit like a Cheddar but also like cheese whiz but in a good way. Pretty snackable, would be great with a good jam and with a red wine. Can't eat a ton at one time because it does dry out the mouth.</t>
+  </si>
+  <si>
+    <t>Very sharp, a bit Cheddary but definitely has that aged Gouda caramely nutty taste going on. A bit of leathery or tobacco-y flavor in there too which is interesting. Would go well with jam or Bourbon. Texture is a bit gummy and chalky which isn't my favorite but has some nice crystals. It's probably too sharp for me to want much in a row, but very nice addition to a diverse cheese board.</t>
+  </si>
+  <si>
+    <t>67f04c10-72b1-11e9-b947-8385855fd8ef</t>
+  </si>
+  <si>
+    <t>Giulia's uncle</t>
+  </si>
+  <si>
+    <t>Giulia's Uncle</t>
+  </si>
+  <si>
+    <t>Homemade with Baggio Evangelista &amp; Joey Ragusa, Jr., along with Carli Opland &amp; Giulia Fragola et al</t>
+  </si>
+  <si>
+    <t>Giulia Fragola et al</t>
+  </si>
+  <si>
+    <t>Pale yellow cheese with thin orange waxy rind. Mild, aged nuttiness - a bit of swiss-like grassy flavor, a bit of brown butter later. Snackable for sure, versatile cheese, does dry out at the edges so seal well.</t>
+  </si>
+  <si>
+    <t>Nutty, milky, Swissy flavor. Very mild, pretty boring tbh. Texture is crumbly &amp; sort of dry (though we bought on sale so maybe a bit old). Tasty enough but unremarkable.</t>
+  </si>
+  <si>
+    <t>FABES</t>
+  </si>
+  <si>
+    <t>Fontina Fontal</t>
+  </si>
+  <si>
+    <t>Pale ivory-ish cheese with a patterned orange waxy rind, firm. Creamy, mildly gummy texture that disintegrates in the mouth. Very mild cheese - a bit nutty &amp; salty but overall neutral, yet not too boring. Would be great paired with any yummy jam.</t>
+  </si>
+  <si>
+    <t>Mild, buttery, with a bit of sharp &amp; tangy finish. Reminds me a bit of an artisinal fancier Muenster. Nice semi firm, semi chewy texture. Not the most exciting, has some "cheese cube" vibes, but super snackable &amp; easy to put away a lot. Probably nice melted on sammie.</t>
+  </si>
+  <si>
+    <t>fabes</t>
+  </si>
+  <si>
+    <t>Dare</t>
+  </si>
+  <si>
+    <t>Roasted Garlic Plant-Based Cheese Wedge</t>
+  </si>
+  <si>
+    <t>Asheville Farmer's Market</t>
+  </si>
+  <si>
+    <t>Pale white soft cheese in a wedge shape but the consistency of cream cheese. Tastes a bit like cream cheese, garlic flavor, also like helluva good French onion dip…yum…addictive. Not very cheese-like, more of a spread, but so tasty. Taste/general: 4.42/5. Vegan: 4.92/5. Cheesiness: 1.3/5.</t>
+  </si>
+  <si>
+    <t>Garlicky, salty, tastes justs like French onion dip. Airy cream cheese texture that melts in mouth. Not a huge fan of flavored cheeses generally (what's it hiding?), but definitely tasty as a spread, &amp; impressive for vegan. General: 3.2/5. Vegan: 4.7/5.</t>
+  </si>
+  <si>
+    <t>dare</t>
+  </si>
+  <si>
+    <t>Glarner Alpkase</t>
+  </si>
+  <si>
+    <t>Firm tan cheese with a gritty light brown rind. Grassy, earthy, salty flavor - kind of salty &amp; a bit funky at the end. Similar taste to a Comte, but less funky &amp; better. Gummyish texture, a bit dry after time.</t>
+  </si>
+  <si>
+    <t>Grassy, Comte-like cheese, but I like it better than most of this style. Center had unique salty sweet flavor. Outer rind funkier, less tasty. Texture good at first, but dried &amp; got a bit gummy.</t>
+  </si>
+  <si>
+    <t>Alp Heuboden</t>
+  </si>
+  <si>
+    <t>glarner-alpkaese-alt-rezent-jaehrig-glarussell-01-768x878</t>
+  </si>
+  <si>
+    <t>Jasper Hill Farm Giftbox</t>
+  </si>
+  <si>
+    <t>Tan firm blocked cheese with a mottled bumpy light brown rind (looks like bread crust). Nutty &amp; caramel flavors, not bery salty, a tiny bit of funk/bark at rind. Gummy/creamy texture, melts well &amp; is delish melted. 1000x better than the last one of these we tried - very snackable now.</t>
+  </si>
+  <si>
+    <t>Nutty, mildly sharp, a bit of caramel, not very salty. Kind of like a cross between Cheddar &amp; Gouda &amp; Comte. Semi hard, a bit gummy, a bit crumbly. Was better first few days, tends to dry out &amp; get gummy.</t>
+  </si>
+  <si>
+    <t>Little Hosmer</t>
+  </si>
+  <si>
+    <t>Soft white/ivory ripe cheese with a soft center &amp; bright white rind. Buttery, mild, salty, mildly herby, bright flavor. Maybe a hint of grass &amp; melon? Brie-like, but a bit more mild &amp; less gooey. Very tasty to me despite the Brie-ness</t>
+  </si>
+  <si>
+    <t>Buttery, salty, a bit sweet, with a mild bit of funk coming in late. Rich Brie-like flavor but also pretty mild. Texture is slightly firmer than average Brie, with nice chewy rind gradient. I could go for slightly more funk but very tasty and snackable.</t>
+  </si>
+  <si>
+    <t>Willoughby</t>
+  </si>
+  <si>
+    <t>Soft ripened round cheese - yellowish gooey inner part with a tan/pinkinsh rind. Buttery as fuck - has a lot of Brie vibes, but darker in color &amp; milder in flavor, not very salty. Excellent with cranberry sauce, on crackers, or jam. This is helping me on my journey to like Brie.</t>
+  </si>
+  <si>
+    <t>Mmm tasty. Very buttery with Brie-like flavors, a bit mushroomy, &amp; a mild funkiness. Super light &amp; airy. Gooey texture &amp; melts in mouth. Very thin rind compared to most Brie, not much chewiness.</t>
+  </si>
+  <si>
+    <t>Barnum Blue</t>
+  </si>
+  <si>
+    <t>Manki Kim &amp; Zoey Song</t>
+  </si>
+  <si>
+    <t>Blue! Stinky! Has a mottled grainy brown thin rind with an ivory &amp; blue/green middle. Firm &amp; crumbly, relatively smooth texture. Salty &amp; funky in the way that goes to the back of the throat. It's not toooo moldy old blue cheese - salt helps balance.</t>
+  </si>
+  <si>
+    <t>031864-jasper-hill-little-hosmer-01</t>
+  </si>
+  <si>
+    <t>Blakesville Creamery</t>
+  </si>
+  <si>
+    <t>Salty, funky blue taste, rich but not overpowering. Really nice subtle flavor compared to more standard Blues. Bit of strange aftertaste though, slightly metallic. Great texture, firmer than other Blues, crumbly &amp; chewy simultaneously. Afternote: their website describes texture as fudgy, which is perfect description.</t>
+  </si>
+  <si>
+    <t>barnum</t>
   </si>
 </sst>
 </file>
@@ -1672,6 +1933,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1971,10 +2236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C16D42-ADCD-457E-8128-5F14C27CE76D}">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="L121" sqref="L121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2299,7 @@
         <v>17</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
@@ -2054,7 +2319,7 @@
         <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="H2" s="3">
         <v>44270</v>
@@ -2194,7 +2459,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>29</v>
@@ -2551,7 +2816,7 @@
         <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="H15" s="3">
         <v>44440</v>
@@ -2808,7 +3073,7 @@
         <v>140</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>66</v>
@@ -2829,7 +3094,7 @@
         <v>4.13</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="L22" s="2">
         <v>4.3</v>
@@ -2840,10 +3105,10 @@
     </row>
     <row r="23" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>79</v>
@@ -2861,19 +3126,19 @@
         <v>44526</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J23" s="2">
         <v>4.67</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L23" s="2">
         <v>3.1</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="72" x14ac:dyDescent="0.3">
@@ -2945,13 +3210,13 @@
         <v>86</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>150</v>
+        <v>572</v>
       </c>
       <c r="H26" s="3">
         <v>44534</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
@@ -2959,10 +3224,10 @@
         <v>83</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>29</v>
@@ -2977,27 +3242,27 @@
         <v>44541</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="J27" s="2">
         <v>3.06</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L27" s="2">
         <v>4.5999999999999996</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>37</v>
@@ -3006,45 +3271,45 @@
         <v>66</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="H28" s="3">
         <v>44555</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J28" s="2">
         <v>3.2</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="L28" s="2">
         <v>3.5</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>29</v>
@@ -3053,42 +3318,42 @@
         <v>105</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H29" s="3">
         <v>44555</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J29" s="2">
         <v>3.65</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L29" s="2">
         <v>3.9</v>
       </c>
       <c r="M29" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>29</v>
@@ -3097,39 +3362,39 @@
         <v>105</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H30" s="3">
         <v>44555</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J30" s="2">
         <v>3.49</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="L30" s="2">
         <v>4</v>
       </c>
       <c r="M30" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>35</v>
@@ -3138,22 +3403,22 @@
         <v>29</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="H31" s="3">
         <v>44555</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J31" s="2">
         <v>4.01</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L31" s="2">
         <v>3</v>
@@ -3164,10 +3429,10 @@
         <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>29</v>
@@ -3182,19 +3447,19 @@
         <v>44562</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J32" s="2">
         <v>4.1100000000000003</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L32" s="2">
         <v>4.0999999999999996</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -3202,16 +3467,16 @@
         <v>13</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>24</v>
@@ -3220,101 +3485,101 @@
         <v>44569</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J33" s="2">
         <v>2.5</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L33" s="2">
         <v>3.9</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>193</v>
+        <v>573</v>
       </c>
       <c r="H34" s="3">
         <v>44570</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J34" s="2">
         <v>4.79</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L34" s="2">
         <v>4.8</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>193</v>
+        <v>573</v>
       </c>
       <c r="H35" s="3">
         <v>44570</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J35" s="2">
         <v>2.4</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L35" s="2">
         <v>2.2000000000000002</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3322,215 +3587,215 @@
         <v>13</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>193</v>
+        <v>573</v>
       </c>
       <c r="H36" s="3">
         <v>44570</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J36" s="2">
         <v>4.57</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L36" s="2">
         <v>2.7</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>209</v>
+        <v>570</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>211</v>
+        <v>571</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>193</v>
+        <v>573</v>
       </c>
       <c r="H37" s="3">
         <v>44570</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J37" s="2">
         <v>4.3899999999999997</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="L37" s="2">
         <v>4.6900000000000004</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>193</v>
+        <v>573</v>
       </c>
       <c r="H38" s="3">
         <v>44570</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J38" s="2">
         <v>3.96</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="L38" s="2">
         <v>2.6</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H39" s="3">
         <v>44575</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="J39" s="2">
         <v>2.6</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="L39" s="2">
         <v>2.6</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H40" s="3">
         <v>44575</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J40" s="2">
         <v>4.7300000000000004</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L40" s="2">
         <v>4.3</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>29</v>
@@ -3539,36 +3804,36 @@
         <v>105</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H41" s="3">
         <v>44575</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="J41" s="2">
         <v>2.11</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="L41" s="2">
         <v>3.4</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>35</v>
@@ -3577,31 +3842,31 @@
         <v>29</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H42" s="3">
         <v>44575</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J42" s="2">
         <v>4.82</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="L42" s="2">
         <v>4.8</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -3609,10 +3874,10 @@
         <v>139</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>66</v>
@@ -3621,36 +3886,36 @@
         <v>28</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H43" s="3">
         <v>44575</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="J43" s="2">
         <v>2.5099999999999998</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="L43" s="2">
         <v>2.4</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>79</v>
@@ -3662,45 +3927,45 @@
         <v>80</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H44" s="3">
         <v>44575</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J44" s="2">
         <v>3.84</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="L44" s="2">
         <v>3.3</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>24</v>
@@ -3709,19 +3974,19 @@
         <v>44592</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J45" s="2">
         <v>2.02</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="L45" s="2">
         <v>3.1</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -3729,7 +3994,7 @@
         <v>71</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>37</v>
@@ -3747,27 +4012,27 @@
         <v>44605</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J46" s="2">
         <v>1.8</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="L46" s="2">
         <v>3.8</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>79</v>
@@ -3785,27 +4050,27 @@
         <v>44612</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="J47" s="2">
         <v>3.1</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="L47" s="2">
         <v>3.7</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>35</v>
@@ -3823,27 +4088,27 @@
         <v>44612</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J48" s="2">
         <v>3.01</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="L48" s="2">
         <v>3.2</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>35</v>
@@ -3852,36 +4117,36 @@
         <v>29</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="H49" s="3">
         <v>44615</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J49" s="2">
         <v>1.98</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="L49" s="2">
         <v>1.3</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>37</v>
@@ -3899,27 +4164,27 @@
         <v>44625</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="J50" s="2">
         <v>3.04</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="L50" s="2">
         <v>2.7</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>37</v>
@@ -3928,7 +4193,7 @@
         <v>29</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>24</v>
@@ -3937,36 +4202,36 @@
         <v>44627</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="J51" s="2">
         <v>3.92</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="L51" s="2">
         <v>3.3</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>106</v>
@@ -3975,33 +4240,33 @@
         <v>44634</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="J52" s="2">
         <v>4.12</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="L52" s="2">
         <v>3.8</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>86</v>
@@ -4013,27 +4278,27 @@
         <v>44639</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="J53" s="2">
         <v>2.89</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="L53" s="2">
         <v>4.3</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>37</v>
@@ -4051,27 +4316,27 @@
         <v>44639</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J54" s="2">
         <v>2</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="L54" s="2">
         <v>3.7</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>37</v>
@@ -4089,13 +4354,13 @@
         <v>44646</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J55" s="2">
         <v>4.3899999999999997</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="L55" s="2">
         <v>4.8499999999999996</v>
@@ -4106,7 +4371,7 @@
         <v>122</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>37</v>
@@ -4124,19 +4389,19 @@
         <v>44646</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="J56" s="2">
         <v>1.6</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="L56" s="2">
         <v>1.4</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -4144,10 +4409,10 @@
         <v>139</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>29</v>
@@ -4162,27 +4427,27 @@
         <v>44646</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="J57" s="2">
         <v>3.01</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="L57" s="2">
         <v>3.3</v>
       </c>
       <c r="M57" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>37</v>
@@ -4200,36 +4465,36 @@
         <v>44646</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="J58" s="2">
         <v>2.4</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="L58" s="2">
         <v>1.8</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C59" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>106</v>
@@ -4239,27 +4504,27 @@
         <v>44654</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J59" s="2">
         <v>2</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="L59" s="2">
         <v>3.6</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>79</v>
@@ -4277,30 +4542,30 @@
         <v>44654</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J60" s="2">
         <v>4.57</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="L60" s="2">
         <v>3.8</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>29</v>
@@ -4315,19 +4580,19 @@
         <v>44654</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="J61" s="2">
         <v>1.4</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L61" s="2">
         <v>1.5</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -4335,16 +4600,16 @@
         <v>139</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>106</v>
@@ -4353,30 +4618,30 @@
         <v>44657</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="J62" s="2">
         <v>4.08</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="L62" s="2">
         <v>3.8</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>29</v>
@@ -4391,19 +4656,19 @@
         <v>44657</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="J63" s="2">
         <v>2.25</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="L63" s="2">
         <v>2</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -4411,7 +4676,7 @@
         <v>110</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>35</v>
@@ -4429,19 +4694,19 @@
         <v>44666</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J64" s="2">
         <v>2</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="L64" s="2">
         <v>2</v>
       </c>
       <c r="M64" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -4449,7 +4714,7 @@
         <v>13</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>37</v>
@@ -4458,28 +4723,28 @@
         <v>29</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="H65" s="3">
         <v>44671</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J65" s="2">
         <v>3.74</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="L65" s="2">
         <v>2.6</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -4487,7 +4752,7 @@
         <v>71</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>37</v>
@@ -4505,19 +4770,19 @@
         <v>44679</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J66" s="2">
         <v>3.49</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="L66" s="2">
         <v>4.0999999999999996</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -4525,7 +4790,7 @@
         <v>139</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>37</v>
@@ -4534,7 +4799,7 @@
         <v>29</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>106</v>
@@ -4543,30 +4808,30 @@
         <v>44683</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="J67" s="2">
         <v>2.04</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L67" s="2">
         <v>2.8</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>29</v>
@@ -4581,27 +4846,27 @@
         <v>44683</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J68" s="2">
         <v>3.69</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="L68" s="2">
         <v>2.9</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>35</v>
@@ -4610,36 +4875,36 @@
         <v>29</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="H69" s="3">
         <v>44690</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="J69" s="2">
         <v>3.12</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="L69" s="2">
         <v>2.6</v>
       </c>
       <c r="M69" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>79</v>
@@ -4654,33 +4919,33 @@
         <v>13</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="H70" s="3">
         <v>44696</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="J70" s="2">
         <v>4.43</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="L70" s="2">
         <v>2.4</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>35</v>
@@ -4698,30 +4963,30 @@
         <v>44696</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J71" s="2">
         <v>2.29</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="L71" s="2">
         <v>2.1</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>29</v>
@@ -4736,19 +5001,19 @@
         <v>44696</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="J72" s="2">
         <v>2.82</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="L72" s="2">
         <v>2.6</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -4756,13 +5021,13 @@
         <v>139</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>28</v>
@@ -4774,19 +5039,19 @@
         <v>44696</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="J73" s="2">
         <v>3.23</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="L73" s="2">
         <v>4.0999999999999996</v>
       </c>
       <c r="M73" s="5" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -4794,7 +5059,7 @@
         <v>83</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>23</v>
@@ -4812,30 +5077,30 @@
         <v>44709</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J74" s="2">
         <v>3.09</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="L74" s="2">
         <v>2.7</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>29</v>
@@ -4844,36 +5109,36 @@
         <v>27</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H75" s="3">
         <v>44709</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="J75" s="2">
         <v>2.34</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="L75" s="2">
         <v>2.2999999999999998</v>
       </c>
       <c r="M75" s="5" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>37</v>
@@ -4885,37 +5150,37 @@
         <v>28</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3">
         <v>44744</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="J76" s="2">
         <v>4.29</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="L76" s="2">
         <v>4.55</v>
       </c>
       <c r="M76" s="5" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>29</v>
@@ -4924,36 +5189,36 @@
         <v>105</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="H77" s="3">
         <v>44744</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="J77" s="2">
         <v>3.21</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="L77" s="2">
         <v>3.8</v>
       </c>
       <c r="M77" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>29</v>
@@ -4968,33 +5233,33 @@
         <v>44751</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J78" s="2">
         <v>2.23</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="L78" s="2">
         <v>1.3</v>
       </c>
       <c r="M78" s="5" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>105</v>
@@ -5006,33 +5271,33 @@
         <v>44751</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="J79" s="2">
         <v>3.19</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="L79" s="2">
         <v>2.8</v>
       </c>
       <c r="M79" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>28</v>
@@ -5044,19 +5309,19 @@
         <v>44753</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="J80" s="2">
         <v>3.48</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="L80" s="2">
         <v>3.7</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -5064,10 +5329,10 @@
         <v>13</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>29</v>
@@ -5082,33 +5347,33 @@
         <v>44752</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J81" s="2">
         <v>2.95</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="L81" s="2">
         <v>1.6</v>
       </c>
       <c r="M81" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>27</v>
@@ -5120,36 +5385,36 @@
         <v>44751</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="J82" s="2">
         <v>4.01</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="L82" s="2">
         <v>3.5</v>
       </c>
       <c r="M82" s="5" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>106</v>
@@ -5158,19 +5423,19 @@
         <v>44751</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="J83" s="2">
         <v>2.15</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="L83" s="2">
         <v>4</v>
       </c>
       <c r="M83" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -5178,10 +5443,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>29</v>
@@ -5196,13 +5461,13 @@
         <v>44752</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="J84" s="2">
         <v>1.97</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="L84" s="2">
         <v>3.5</v>
@@ -5210,10 +5475,10 @@
     </row>
     <row r="85" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>37</v>
@@ -5231,27 +5496,27 @@
         <v>44760</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="J85" s="2">
         <v>1.76</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="L85" s="2">
         <v>1.8</v>
       </c>
       <c r="M85" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>35</v>
@@ -5269,19 +5534,19 @@
         <v>44760</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="J86" s="2">
         <v>2.16</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="L86" s="2">
         <v>2.6</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -5289,7 +5554,7 @@
         <v>13</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>79</v>
@@ -5307,19 +5572,19 @@
         <v>44765</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="J87" s="2">
         <v>3.23</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="L87" s="2">
         <v>2.4</v>
       </c>
       <c r="M87" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="144" x14ac:dyDescent="0.3">
@@ -5342,19 +5607,19 @@
         <v>58</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H88" s="3">
         <v>44773</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="J88" s="2">
         <v>4.67</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="L88" s="2">
         <v>4.5999999999999996</v>
@@ -5368,7 +5633,7 @@
         <v>139</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>128</v>
@@ -5386,27 +5651,27 @@
         <v>44773</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="J89" s="2">
         <v>4.03</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="L89" s="2">
         <v>4</v>
       </c>
       <c r="M89" s="5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>35</v>
@@ -5424,30 +5689,30 @@
         <v>44773</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J90" s="2">
         <v>4.01</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="L90" s="2">
         <v>3.8</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>66</v>
@@ -5456,36 +5721,36 @@
         <v>86</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="H91" s="3">
         <v>44786</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="J91" s="2">
         <v>2.0299999999999998</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="L91" s="2">
         <v>2.4</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>29</v>
@@ -5500,30 +5765,30 @@
         <v>44788</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="J92" s="2">
         <v>2.2799999999999998</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="L92" s="2">
         <v>1.7</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>29</v>
@@ -5538,27 +5803,27 @@
         <v>44789</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="J93" s="2">
         <v>2.52</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="L93" s="2">
         <v>2.7</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>37</v>
@@ -5576,30 +5841,30 @@
         <v>44789</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J94" s="2">
         <v>3.18</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="L94" s="2">
         <v>3.3</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>29</v>
@@ -5614,27 +5879,27 @@
         <v>44789</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="J95" s="2">
         <v>2.06</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="L95" s="2">
         <v>4.0999999999999996</v>
       </c>
       <c r="M95" s="5" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>37</v>
@@ -5646,33 +5911,33 @@
         <v>105</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H96" s="3">
         <v>44808</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="J96" s="2">
         <v>2.38</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="L96" s="2">
         <v>3.4</v>
       </c>
       <c r="M96" s="5" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>37</v>
@@ -5684,36 +5949,36 @@
         <v>80</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H97" s="3">
         <v>44808</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="J97" s="2">
         <v>3.91</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="L97" s="2">
         <v>3.5</v>
       </c>
       <c r="M97" s="5" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>29</v>
@@ -5722,33 +5987,33 @@
         <v>124</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H98" s="3">
         <v>44808</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="J98" s="2">
         <v>1.53</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="L98" s="2">
         <v>0.8</v>
       </c>
       <c r="M98" s="5" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>37</v>
@@ -5760,69 +6025,859 @@
         <v>28</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H99" s="3">
         <v>44821</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="J99" s="2">
         <v>2.4500000000000002</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="L99" s="2">
         <v>3.6</v>
       </c>
       <c r="M99" s="5" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" ht="144" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>517</v>
-      </c>
       <c r="G100" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H100" s="3">
         <v>44821</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="J100" s="2">
         <v>2.83</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="L100" s="2">
         <v>1.8</v>
       </c>
       <c r="M100" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="N100" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H101" s="3">
+        <v>44821</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="J101" s="2">
+        <v>3.67</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="L101" s="2">
+        <v>4</v>
+      </c>
+      <c r="M101" s="5" t="s">
         <v>520</v>
+      </c>
+      <c r="N101" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H102" s="3">
+        <v>44821</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="J102" s="2">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="L102" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M102" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="N102" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H103" s="3">
+        <v>44821</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="J103" s="2">
+        <v>2.82</v>
+      </c>
+      <c r="K103" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="L103" s="2">
+        <v>3</v>
+      </c>
+      <c r="M103" s="5" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H104" s="3">
+        <v>44835</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="J104" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="L104" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H105" s="3">
+        <v>44835</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="J105" s="2">
+        <v>3.92</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="L105" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="M105" s="5" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H106" s="3">
+        <v>44835</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="J106" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="L106" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="M106" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H107" s="3">
+        <v>44843</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="J107" s="2">
+        <v>1.86</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="L107" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="M107" s="5" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H108" s="3">
+        <v>44843</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="J108" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="L108" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M108" s="5" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H109" s="3">
+        <v>44843</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="J109" s="2">
+        <v>3.97</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="L109" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M109" s="5" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H110" s="3">
+        <v>44849</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="J110" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="K110" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="L110" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="M110" s="5" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H111" s="3">
+        <v>44849</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="J111" s="2">
+        <v>3.78</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="L111" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="M111" s="5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H112" s="3">
+        <v>44856</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="J112" s="2">
+        <v>4.42</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L112" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="M112" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H113" s="3">
+        <v>44860</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="J113" s="2">
+        <v>3.74</v>
+      </c>
+      <c r="K113" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="L113" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="M113" s="5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H114" s="3">
+        <v>44860</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="J114" s="2">
+        <v>3.39</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="L114" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="M114" s="5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H115" s="3">
+        <v>44860</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="J115" s="2">
+        <v>3.04</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="L115" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="M115" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H116" s="3">
+        <v>44872</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="J116" s="2">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="L116" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="M116" s="5" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H117" s="3">
+        <v>44887</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="J117" s="2">
+        <v>4.34</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="L117" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="M117" s="5" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H118" s="3">
+        <v>44887</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="J118" s="2">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="L118" s="2">
+        <v>3.95</v>
+      </c>
+      <c r="M118" s="5" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H119" s="3">
+        <v>44887</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="J119" s="2">
+        <v>4.47</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="L119" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="M119" s="5" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="H120" s="3">
+        <v>44889</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="J120" s="2">
+        <v>2.81</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="L120" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M120" s="5" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>